<commit_message>
Se suben cambios completados modulo de liquidacion para laboratorios y que la logica se la puede escalar para los demas  servicios, funciona correctamente
</commit_message>
<xml_diff>
--- a/data/excel/TARIFAS CLINICA FATIMA GLICOL.xlsx
+++ b/data/excel/TARIFAS CLINICA FATIMA GLICOL.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Descargas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\9. NOVENO SEMESTRE\PRACTICA\proyecto-clinica-fatima\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -476,7 +476,7 @@
     <t>LABORATORIO</t>
   </si>
   <si>
-    <t>GLICOL Y CYA</t>
+    <t>GLICOL Y CIA</t>
   </si>
 </sst>
 </file>
@@ -923,8 +923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>